<commit_message>
Carga de personas y equipos lista
Carga de personas y equipos lista
</commit_message>
<xml_diff>
--- a/backend/Carga.xlsx
+++ b/backend/Carga.xlsx
@@ -7,16 +7,32 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Dep1" sheetId="1" r:id="rId1"/>
+    <sheet name="futbol" sheetId="1" r:id="rId1"/>
+    <sheet name="futbol varones" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Hello, world!</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>rut</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>emergency_phone</t>
   </si>
 </sst>
 </file>
@@ -348,15 +364,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Cálculo de puntajes
Las puntuaciones ahora se muestran correctamente en la página
</commit_message>
<xml_diff>
--- a/backend/Carga.xlsx
+++ b/backend/Carga.xlsx
@@ -7,15 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="futbol" sheetId="1" r:id="rId1"/>
-    <sheet name="futbol varones" sheetId="2" r:id="rId2"/>
+    <sheet name="Personas" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>nombre</t>
   </si>
@@ -393,37 +392,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
correciones antes de validacion con usuarios
correciones antes de validacion con usuarios
</commit_message>
<xml_diff>
--- a/backend/Carga.xlsx
+++ b/backend/Carga.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Personas" sheetId="1" r:id="rId1"/>
+    <sheet name="futbol varones" sheetId="1" r:id="rId1"/>
+    <sheet name="futbol damas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>nombre</t>
   </si>
@@ -392,4 +393,37 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>